<commit_message>
Update latest example sheets
</commit_message>
<xml_diff>
--- a/sheets/match_result.xlsx
+++ b/sheets/match_result.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectData\PythonProject\LiquipediaOsuContributeHelper\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B26EAE2-42D0-4CF8-A27C-5E2BCA9891FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB280613-2263-4BC2-9487-E813A5F061BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1190" yWindow="1430" windowWidth="22160" windowHeight="11470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4600" yWindow="0" windowWidth="21000" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>BID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,6 +76,58 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>MATCH LINK</t>
+  </si>
+  <si>
+    <t>#7</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>#8</t>
+  </si>
+  <si>
+    <t>#14</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>#9</t>
+  </si>
+  <si>
+    <t>#10</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#12</t>
+  </si>
+  <si>
+    <t>#13</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>#11</t>
+  </si>
+  <si>
+    <t>#15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>RC1</t>
   </si>
   <si>
@@ -93,6 +146,9 @@
     <t>RC6</t>
   </si>
   <si>
+    <t>RC7</t>
+  </si>
+  <si>
     <t>HB1</t>
   </si>
   <si>
@@ -111,26 +167,20 @@
     <t>LN3</t>
   </si>
   <si>
+    <t>LN4</t>
+  </si>
+  <si>
     <t>SV1</t>
   </si>
   <si>
     <t>SV2</t>
-  </si>
-  <si>
-    <t>TB1</t>
-  </si>
-  <si>
-    <t>RC7</t>
-  </si>
-  <si>
-    <t>LN4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,19 +256,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9"/>
-      <color rgb="FFC38AF9"/>
+      <color rgb="FFB5B5FC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FFC38AF9"/>
+      <sz val="9"/>
+      <color rgb="FF8B8BE6"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,12 +314,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF201037"/>
+        <fgColor rgb="FFB46001"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8CDDFA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB86014"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1F1F47"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -253,73 +346,50 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color rgb="FF5C300A"/>
+      </left>
       <right style="medium">
-        <color rgb="FF000000"/>
+        <color rgb="FFB86014"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color rgb="FF5C300A"/>
+      </top>
       <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color rgb="FF5C300A"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color rgb="FF5C300A"/>
+      </left>
       <right style="medium">
-        <color rgb="FF000000"/>
+        <color rgb="FFB46001"/>
       </right>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
+      <top style="medium">
+        <color rgb="FF68310B"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF68310B"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
+      <left style="medium">
+        <color rgb="FF68310B"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF68310B"/>
+      </top>
       <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="mediumDashed">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="mediumDashed">
-        <color rgb="FF000000"/>
+        <color rgb="FF68310B"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
@@ -328,8 +398,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -345,11 +416,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -360,35 +452,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="2" xr:uid="{7E0D03F8-8550-474D-A3A7-3F47D175B4FE}"/>
     <cellStyle name="常规 3" xfId="1" xr:uid="{8210E84D-A243-4508-A258-2B507FDCAAA6}"/>
+    <cellStyle name="超链接" xfId="4" builtinId="8"/>
     <cellStyle name="超链接 2" xfId="3" xr:uid="{45425DC9-A299-4809-AED5-D482CC038F96}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -669,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -693,18 +762,18 @@
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="16"/>
+      <c r="E2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="H2" s="10" t="s">
+      <c r="F2" s="16"/>
+      <c r="H2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -721,275 +790,302 @@
       <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="12" t="s">
-        <v>8</v>
+      <c r="H3" s="18"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="14" t="s">
+        <v>25</v>
       </c>
       <c r="C4" s="15">
-        <v>3763263</v>
+        <v>4376111</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="J4" s="6">
-        <v>103862590</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="12" t="s">
-        <v>9</v>
+      <c r="J4" s="12">
+        <v>111442399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="C5" s="15">
-        <v>3671281</v>
+        <v>4373684</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-      <c r="J5" s="6">
-        <v>103872600</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="12" t="s">
-        <v>10</v>
+      <c r="J5" s="12">
+        <v>111444281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="C6" s="15">
-        <v>1762209</v>
-      </c>
-      <c r="J6" s="6">
-        <v>103874849</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="12" t="s">
-        <v>11</v>
+        <v>4373833</v>
+      </c>
+      <c r="J6" s="12">
+        <v>111444684</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="C7" s="15">
-        <v>3756153</v>
-      </c>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="12" t="s">
-        <v>12</v>
+        <v>4347612</v>
+      </c>
+      <c r="J7" s="12">
+        <v>111444745</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="C8" s="15">
-        <v>3513548</v>
-      </c>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="12" t="s">
-        <v>13</v>
+        <v>4383861</v>
+      </c>
+      <c r="J8" s="12">
+        <v>111444611</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="C9" s="15">
-        <v>3783809</v>
-      </c>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="16">
-        <v>3331564</v>
-      </c>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="17">
-        <v>3793096</v>
-      </c>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="12" t="s">
-        <v>15</v>
+        <v>4376216</v>
+      </c>
+      <c r="J9" s="12">
+        <v>111445294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="15">
+        <v>4375874</v>
+      </c>
+      <c r="J10" s="1">
+        <v>111445603</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="15">
+        <v>4383872</v>
+      </c>
+      <c r="J11" s="12">
+        <v>111446109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="C12" s="15">
-        <v>3595933</v>
-      </c>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="16">
-        <v>3790784</v>
-      </c>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="12" t="s">
-        <v>17</v>
+        <v>4339954</v>
+      </c>
+      <c r="J12" s="12">
+        <v>111446273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="15">
+        <v>4370711</v>
+      </c>
+      <c r="J13" s="12">
+        <v>111446197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="C14" s="15">
-        <v>3792661</v>
-      </c>
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="12" t="s">
-        <v>18</v>
+        <v>3588685</v>
+      </c>
+      <c r="J14" s="13">
+        <v>111462023</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="C15" s="15">
-        <v>3629447</v>
-      </c>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="12" t="s">
-        <v>19</v>
+        <v>3870447</v>
+      </c>
+      <c r="J15" s="13">
+        <v>111462013</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="C16" s="15">
-        <v>3792636</v>
-      </c>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="2:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="18">
-        <v>3592063</v>
-      </c>
-      <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="2:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="12" t="s">
-        <v>20</v>
+        <v>4382915</v>
+      </c>
+      <c r="J16" s="13">
+        <v>111461970</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="15">
+        <v>3998427</v>
+      </c>
+      <c r="J17" s="12">
+        <v>111462057</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="C18" s="15">
-        <v>3793332</v>
+        <v>4376223</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="2:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="16">
-        <v>3793380</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J18" s="12">
+        <v>111462950</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="15">
+        <v>4383864</v>
+      </c>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="19">
-        <v>3793375</v>
-      </c>
-      <c r="J20" s="8"/>
-    </row>
-    <row r="21" spans="2:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="J21" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>2429180</v>
+      </c>
+      <c r="J20" s="12"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H22" s="6"/>
-      <c r="J22" s="8"/>
+      <c r="J22" s="12"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H23" s="6"/>
-      <c r="J23" s="8"/>
+      <c r="J23" s="13"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H24" s="6"/>
-      <c r="J24" s="7"/>
+      <c r="J24" s="13"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H25" s="6"/>
-      <c r="J25" s="7"/>
+      <c r="J25" s="13"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H26" s="6"/>
-      <c r="J26" s="7"/>
+      <c r="J26" s="13"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H27" s="6"/>
-      <c r="J27" s="7"/>
+      <c r="J27" s="13"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H28" s="6"/>
-      <c r="J28" s="7"/>
+      <c r="J28" s="13"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H29" s="6"/>
-      <c r="J29" s="7"/>
+      <c r="J29" s="13"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H30" s="6"/>
-      <c r="J30" s="7"/>
+      <c r="J30" s="13"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H31" s="6"/>
-      <c r="J31" s="7"/>
+      <c r="J31" s="13"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H32" s="6"/>
-      <c r="J32" s="7"/>
+      <c r="J32" s="13"/>
     </row>
     <row r="33" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H33" s="6"/>
-      <c r="J33" s="7"/>
+      <c r="J33" s="13"/>
     </row>
     <row r="34" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H34" s="6"/>
-      <c r="J34" s="7"/>
+      <c r="J34" s="13"/>
     </row>
     <row r="35" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H35" s="6"/>
-      <c r="J35" s="7"/>
+      <c r="J35" s="13"/>
     </row>
     <row r="36" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H36" s="6"/>
-      <c r="J36" s="7"/>
+      <c r="J36" s="13"/>
     </row>
     <row r="37" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H37" s="6"/>
-      <c r="J37" s="7"/>
+      <c r="J37" s="13"/>
     </row>
     <row r="38" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H38" s="6"/>
-      <c r="J38" s="7"/>
+      <c r="J38" s="13"/>
     </row>
     <row r="39" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H39" s="6"/>
-      <c r="J39" s="7"/>
+      <c r="J39" s="13"/>
     </row>
     <row r="40" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H40" s="6"/>
-      <c r="J40" s="7"/>
+      <c r="J40" s="13"/>
     </row>
     <row r="41" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H41" s="6"/>
-      <c r="J41" s="7"/>
+      <c r="J41" s="13"/>
     </row>
     <row r="42" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H42" s="6"/>
-      <c r="J42" s="7"/>
+      <c r="J42" s="12"/>
     </row>
     <row r="43" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H43" s="6"/>
+      <c r="J43" s="12"/>
     </row>
     <row r="44" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H44" s="6"/>
+      <c r="J44" s="12"/>
     </row>
     <row r="45" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H45" s="6"/>
+      <c r="J45" s="12"/>
     </row>
     <row r="46" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H46" s="6"/>
+      <c r="J46" s="12"/>
     </row>
     <row r="47" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H47" s="6"/>
+      <c r="J47" s="12"/>
     </row>
     <row r="48" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H48" s="6"/>
@@ -1527,4 +1623,161 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A0749C-2422-40D8-9A03-AF8E0E60A503}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>111333367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>111349046</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>111349077</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>111349240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>111349880</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>111349895</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>111349867</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>111350097</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>111350197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>111350658</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>111350669</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>111363870</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>111367198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>111369284</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://osu.ppy.sh/community/matches/111333367" xr:uid="{5E980CF9-D1CC-493B-B65D-11149662A8BD}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://osu.ppy.sh/community/matches/111349046" xr:uid="{71BB6D0B-4652-4D54-A97F-5A393776760D}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://osu.ppy.sh/mp/111349077" xr:uid="{C76DF6F9-B675-4B41-82F5-482A1B1B1802}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://osu.ppy.sh/community/matches/111349240" xr:uid="{7818EFB5-8393-49FC-B8E4-389CAA31ABD3}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://osu.ppy.sh/community/matches/111349880" xr:uid="{3F00BABF-79F2-4FDC-B9B6-9EB6453F1C99}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://osu.ppy.sh/community/matches/111349895" xr:uid="{9D76FC0A-7E57-4D8C-AE7E-8CF9AC9570FF}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://osu.ppy.sh/community/matches/111349867" xr:uid="{59DC2BC7-34FF-40D0-B762-DC8FC7811857}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://osu.ppy.sh/community/matches/111350097" xr:uid="{5D2BF658-A0AF-4A7B-AC2D-D7600602EB3F}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://osu.ppy.sh/community/matches/111350197" xr:uid="{3758B910-A34E-4FD6-A831-C0BBDD79FE39}"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://osu.ppy.sh/community/matches/111350658" xr:uid="{07467001-38C2-4029-875F-D922B91B7C21}"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://osu.ppy.sh/community/matches/111350669" xr:uid="{F4500163-E72F-428D-BA1C-BDB3929986B5}"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://osu.ppy.sh/community/matches/111363870" xr:uid="{DE32F630-8B6E-44C4-B1D0-27DE32B75092}"/>
+    <hyperlink ref="A15" r:id="rId13" display="https://osu.ppy.sh/mp/111367198" xr:uid="{98E3B5BB-9306-4568-8EFD-95BE886E5821}"/>
+    <hyperlink ref="A16" r:id="rId14" display="https://osu.ppy.sh/community/matches/111369284" xr:uid="{474A18EE-818A-4541-BC32-6D5014337761}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add: settings that allowed swap team results.
</commit_message>
<xml_diff>
--- a/sheets/match_result.xlsx
+++ b/sheets/match_result.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectData\PythonProject\LiquipediaOsuContributeHelper\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB280613-2263-4BC2-9487-E813A5F061BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FB823F-FCDF-43AC-8CFB-842DA75BA653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4600" yWindow="0" windowWidth="21000" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2770" yWindow="1740" windowWidth="21010" windowHeight="12670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Options" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>BID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -128,59 +129,82 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RC1</t>
-  </si>
-  <si>
-    <t>RC2</t>
-  </si>
-  <si>
-    <t>RC3</t>
-  </si>
-  <si>
-    <t>RC4</t>
-  </si>
-  <si>
-    <t>RC5</t>
-  </si>
-  <si>
-    <t>RC6</t>
-  </si>
-  <si>
-    <t>RC7</t>
-  </si>
-  <si>
-    <t>HB1</t>
-  </si>
-  <si>
-    <t>HB2</t>
-  </si>
-  <si>
-    <t>HB3</t>
-  </si>
-  <si>
-    <t>LN1</t>
-  </si>
-  <si>
-    <t>LN2</t>
-  </si>
-  <si>
-    <t>LN3</t>
-  </si>
-  <si>
-    <t>LN4</t>
-  </si>
-  <si>
-    <t>SV1</t>
-  </si>
-  <si>
-    <t>SV2</t>
+    <t>FM3</t>
+  </si>
+  <si>
+    <t>FM4</t>
+  </si>
+  <si>
+    <t>FM5</t>
+  </si>
+  <si>
+    <t>FM6</t>
+  </si>
+  <si>
+    <t>FM7</t>
+  </si>
+  <si>
+    <t>FM8</t>
+  </si>
+  <si>
+    <t>FM9</t>
+  </si>
+  <si>
+    <t>FM10</t>
+  </si>
+  <si>
+    <t>FM11</t>
+  </si>
+  <si>
+    <t>FM12</t>
+  </si>
+  <si>
+    <t>Settings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Means all matches in mplink are played 
+in old style (Team1 = Blue, Team2 = Red)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Swap Teams?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bool Values</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FM1</t>
+  </si>
+  <si>
+    <t>FM2</t>
+  </si>
+  <si>
+    <t>FM13</t>
+  </si>
+  <si>
+    <t>FM14</t>
+  </si>
+  <si>
+    <t>FM15</t>
+  </si>
+  <si>
+    <t>FM16</t>
+  </si>
+  <si>
+    <t>FM17</t>
+  </si>
+  <si>
+    <t>FM18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,8 +316,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,6 +366,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF1F1F47"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,7 +439,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -434,9 +473,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -450,6 +486,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -736,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K222"/>
+  <dimension ref="A1:Q222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -751,9 +802,15 @@
     <col min="9" max="9" width="2.58203125" style="3" customWidth="1"/>
     <col min="10" max="10" width="20.58203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="2.58203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="3" customWidth="1"/>
+    <col min="13" max="13" width="23.58203125" customWidth="1"/>
+    <col min="14" max="14" width="2.08203125" customWidth="1"/>
+    <col min="15" max="15" width="7.25" customWidth="1"/>
+    <col min="16" max="16" width="3.1640625" customWidth="1"/>
+    <col min="17" max="17" width="2.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -761,23 +818,30 @@
       <c r="F1" s="2"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="E2" s="16" t="s">
+      <c r="C2" s="15"/>
+      <c r="E2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="H2" s="17" t="s">
+      <c r="F2" s="15"/>
+      <c r="H2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L2" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
@@ -790,298 +854,307 @@
       <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="15">
-        <v>4376111</v>
+      <c r="H3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="6">
+        <v>486159</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="J4" s="12">
-        <v>111442399</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="15">
-        <v>4373684</v>
+      <c r="J4" s="18">
+        <v>22428318</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" s="19"/>
+    </row>
+    <row r="5" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="6">
+        <v>844168</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-      <c r="J5" s="12">
-        <v>111444281</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
+      <c r="J5" s="18">
+        <v>22424367</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="6">
+        <v>851023</v>
+      </c>
+      <c r="J6" s="18">
+        <v>22459042</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="6">
+        <v>833293</v>
+      </c>
+      <c r="J7" s="22">
+        <v>22457102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="15">
-        <v>4373833</v>
-      </c>
-      <c r="J6" s="12">
-        <v>111444684</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
+      <c r="C8" s="6">
+        <v>678816</v>
+      </c>
+      <c r="J8" s="1">
+        <v>22643409</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="15">
-        <v>4347612</v>
-      </c>
-      <c r="J7" s="12">
-        <v>111444745</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
+      <c r="C9" s="6">
+        <v>583877</v>
+      </c>
+      <c r="J9" s="22"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="15">
-        <v>4383861</v>
-      </c>
-      <c r="J8" s="12">
-        <v>111444611</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
+      <c r="C10" s="6">
+        <v>760453</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="15">
-        <v>4376216</v>
-      </c>
-      <c r="J9" s="12">
-        <v>111445294</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
+      <c r="C11" s="6">
+        <v>884617</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="15">
-        <v>4375874</v>
-      </c>
-      <c r="J10" s="1">
-        <v>111445603</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="14" t="s">
+      <c r="C12" s="6">
+        <v>819643</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="15">
-        <v>4383872</v>
-      </c>
-      <c r="J11" s="12">
-        <v>111446109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
+      <c r="C13" s="6">
+        <v>759704</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="15">
-        <v>4339954</v>
-      </c>
-      <c r="J12" s="12">
-        <v>111446273</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="14" t="s">
+      <c r="C14" s="6">
+        <v>329057</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="15">
-        <v>4370711</v>
-      </c>
-      <c r="J13" s="12">
-        <v>111446197</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="15">
-        <v>3588685</v>
-      </c>
-      <c r="J14" s="13">
-        <v>111462023</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="15">
-        <v>3870447</v>
-      </c>
-      <c r="J15" s="13">
-        <v>111462013</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="15">
-        <v>4382915</v>
-      </c>
-      <c r="J16" s="13">
-        <v>111461970</v>
-      </c>
+      <c r="C15" s="6">
+        <v>698696</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="6">
+        <v>871018</v>
+      </c>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="15">
-        <v>3998427</v>
-      </c>
-      <c r="J17" s="12">
-        <v>111462057</v>
-      </c>
+      <c r="B17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="6">
+        <v>888793</v>
+      </c>
+      <c r="J17" s="18"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="15">
-        <v>4376223</v>
+      <c r="B18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="6">
+        <v>890961</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="J18" s="12">
-        <v>111462950</v>
-      </c>
+      <c r="J18" s="18"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="15">
-        <v>4383864</v>
-      </c>
-      <c r="J19" s="12"/>
+      <c r="B19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="14">
+        <v>723703</v>
+      </c>
+      <c r="J19" s="18"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20">
+        <v>323070</v>
+      </c>
+      <c r="J20" s="18"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21">
+        <v>431300</v>
+      </c>
+      <c r="J21" s="18"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
         <v>8</v>
       </c>
-      <c r="C20">
-        <v>2429180</v>
-      </c>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>891715</v>
+      </c>
       <c r="H22" s="6"/>
-      <c r="J22" s="12"/>
+      <c r="J22" s="18"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H23" s="6"/>
-      <c r="J23" s="13"/>
+      <c r="J23" s="18"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H24" s="6"/>
-      <c r="J24" s="13"/>
+      <c r="J24" s="18"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H25" s="6"/>
-      <c r="J25" s="13"/>
+      <c r="J25" s="18"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H26" s="6"/>
-      <c r="J26" s="13"/>
+      <c r="J26" s="18"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H27" s="6"/>
-      <c r="J27" s="13"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H28" s="6"/>
-      <c r="J28" s="13"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H29" s="6"/>
-      <c r="J29" s="13"/>
+      <c r="J29" s="18"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H30" s="6"/>
-      <c r="J30" s="13"/>
+      <c r="J30" s="18"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H31" s="6"/>
-      <c r="J31" s="13"/>
+      <c r="J31" s="18"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H32" s="6"/>
-      <c r="J32" s="13"/>
+      <c r="J32" s="18"/>
     </row>
     <row r="33" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H33" s="6"/>
-      <c r="J33" s="13"/>
+      <c r="J33" s="18"/>
     </row>
     <row r="34" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H34" s="6"/>
-      <c r="J34" s="13"/>
+      <c r="J34" s="18"/>
     </row>
     <row r="35" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H35" s="6"/>
-      <c r="J35" s="13"/>
+      <c r="J35" s="18"/>
     </row>
     <row r="36" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H36" s="6"/>
-      <c r="J36" s="13"/>
+      <c r="J36" s="18"/>
     </row>
     <row r="37" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H37" s="6"/>
-      <c r="J37" s="13"/>
+      <c r="J37" s="18"/>
     </row>
     <row r="38" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H38" s="6"/>
-      <c r="J38" s="13"/>
+      <c r="J38" s="18"/>
     </row>
     <row r="39" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H39" s="6"/>
-      <c r="J39" s="13"/>
+      <c r="J39" s="18"/>
     </row>
     <row r="40" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H40" s="6"/>
-      <c r="J40" s="13"/>
+      <c r="J40" s="18"/>
     </row>
     <row r="41" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H41" s="6"/>
-      <c r="J41" s="13"/>
     </row>
     <row r="42" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H42" s="6"/>
-      <c r="J42" s="12"/>
     </row>
     <row r="43" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H43" s="6"/>
-      <c r="J43" s="12"/>
     </row>
     <row r="44" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H44" s="6"/>
-      <c r="J44" s="12"/>
     </row>
     <row r="45" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H45" s="6"/>
-      <c r="J45" s="12"/>
     </row>
     <row r="46" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H46" s="6"/>
-      <c r="J46" s="12"/>
     </row>
     <row r="47" spans="8:10" x14ac:dyDescent="0.3">
       <c r="H47" s="6"/>
@@ -1613,19 +1686,66 @@
       <c r="H222" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="L5:P6"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="L2:P3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2D3DF8A5-3462-4D9C-917B-A0FDACE6A8C7}">
+          <x14:formula1>
+            <xm:f>Options!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>O4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D3A107-E43C-4490-95DA-4D97364B7381}">
+  <dimension ref="B1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A0749C-2422-40D8-9A03-AF8E0E60A503}">
   <dimension ref="A1:B16"/>
   <sheetViews>

</xml_diff>